<commit_message>
Updating sizing of figures, merging figures of economic impact
</commit_message>
<xml_diff>
--- a/results/intro_table1.xlsx
+++ b/results/intro_table1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\3. PhD\WQE\WQE II\gmh_econ\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6393A674-B186-47A1-B58E-F488EB6A9448}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5262BD2-535B-4A97-8C41-F05358650440}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="2100" windowWidth="19005" windowHeight="13365" xr2:uid="{6C2D4880-6826-4C0E-8266-9CE23D5A6433}"/>
+    <workbookView xWindow="5040" yWindow="2100" windowWidth="19425" windowHeight="10425" activeTab="1" xr2:uid="{6C2D4880-6826-4C0E-8266-9CE23D5A6433}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Value of a statistical life</t>
   </si>
@@ -64,6 +65,24 @@
   </si>
   <si>
     <t>Share from mental illness</t>
+  </si>
+  <si>
+    <t>1x GDP per capita</t>
+  </si>
+  <si>
+    <t>3x GDP per capita</t>
+  </si>
+  <si>
+    <t>High income</t>
+  </si>
+  <si>
+    <t>Upper-middle income</t>
+  </si>
+  <si>
+    <t>Lower-middle income</t>
+  </si>
+  <si>
+    <t>Low income</t>
   </si>
 </sst>
 </file>
@@ -73,13 +92,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -98,11 +123,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -119,18 +162,37 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D1FAA6-632F-48AF-99AB-834A48E4C576}">
   <dimension ref="A2:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J17" sqref="I15:J17"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,11 +529,11 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>5</v>
@@ -517,7 +579,7 @@
         <v>2.4929999999999999</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="6">
+      <c r="G4" s="8">
         <v>16.3</v>
       </c>
       <c r="H4" s="4"/>
@@ -548,7 +610,7 @@
         <v>6.0460000000000003</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4">
         <f>K5*L5</f>
@@ -587,11 +649,11 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
@@ -621,29 +683,29 @@
         <v>2010</v>
       </c>
       <c r="B15" s="4"/>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <f>C4*$B$10/$B$9</f>
         <v>0.96388793009522566</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <f t="shared" ref="D15:E16" si="0">D4*$B$10/$B$9</f>
         <v>1.9570555664509384</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <f>E4*$B$10/$B$9</f>
         <v>2.9197723082957441</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8">
+      <c r="F15" s="6"/>
+      <c r="G15" s="9">
         <f>G4*$B$10/$B$9</f>
         <v>19.090368481837398</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9">
+      <c r="H15" s="7"/>
+      <c r="I15" s="7">
         <f>I4*$B$10/$B$9</f>
         <v>1.5718579150366601</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="7">
         <f>I15*3</f>
         <v>4.71557374510998</v>
       </c>
@@ -653,51 +715,51 @@
         <v>2030</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f>C5*$B$10/$B$9</f>
         <v>2.3365205595868472</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <f t="shared" si="0"/>
         <v>4.7444836024492822</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <f t="shared" si="0"/>
         <v>7.0810041620361295</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9">
+      <c r="F16" s="6"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7">
         <f>I5*$B$10/$B$9</f>
         <v>2.9176922996015819</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16" s="7">
         <f>I16*3</f>
         <v>8.7530768988047463</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f>GEOMEAN(C15:C16)</f>
         <v>1.5007144851053795</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <f t="shared" ref="D17:E17" si="1">GEOMEAN(D15:D16)</f>
         <v>3.0471655754337617</v>
       </c>
-      <c r="E17" s="7">
-        <f t="shared" si="1"/>
+      <c r="E17" s="6">
+        <f>GEOMEAN(E15:E16)</f>
         <v>4.5469682060951335</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="7">
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6">
         <f t="shared" ref="I17:J17" si="2">GEOMEAN(I15:I16)</f>
         <v>2.1415409720036318</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <f t="shared" si="2"/>
         <v>6.4246229160108959</v>
       </c>
@@ -711,4 +773,187 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6BEA9A-A145-4DD6-A3EC-70A58E78C38F}">
+  <dimension ref="B3:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="6" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2010</v>
+      </c>
+      <c r="D4">
+        <v>2030</v>
+      </c>
+      <c r="E4">
+        <v>2010</v>
+      </c>
+      <c r="F4">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <f>C13/$C$17*$C$10</f>
+        <v>1.0158823529411765</v>
+      </c>
+      <c r="D5" s="16">
+        <f>D13/$D$17*$D$10</f>
+        <v>2.1401242236024842</v>
+      </c>
+      <c r="E5" s="16">
+        <f>C5*3</f>
+        <v>3.0476470588235296</v>
+      </c>
+      <c r="F5" s="16">
+        <f>D5*3</f>
+        <v>6.4203726708074527</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="16">
+        <f t="shared" ref="C6:C8" si="0">C14/$C$17*$C$10</f>
+        <v>0.3509411764705882</v>
+      </c>
+      <c r="D6" s="16">
+        <f t="shared" ref="D6:D8" si="1">D14/$D$17*$D$10</f>
+        <v>1.9055900621118012</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" ref="E6:E8" si="2">C6*3</f>
+        <v>1.0528235294117647</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" ref="F6:F8" si="3">D6*3</f>
+        <v>5.7167701863354035</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="16">
+        <f t="shared" si="0"/>
+        <v>0.16623529411764706</v>
+      </c>
+      <c r="D7" s="16">
+        <f t="shared" si="1"/>
+        <v>0.586335403726708</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="2"/>
+        <v>0.49870588235294122</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="3"/>
+        <v>1.7590062111801239</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="16">
+        <f t="shared" si="0"/>
+        <v>3.6941176470588234E-2</v>
+      </c>
+      <c r="D8" s="16">
+        <f t="shared" si="1"/>
+        <v>0.1172670807453416</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="2"/>
+        <v>0.11082352941176471</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="3"/>
+        <v>0.35180124223602482</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="11">
+        <v>1.57</v>
+      </c>
+      <c r="D10" s="14">
+        <v>4.72</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2.92</v>
+      </c>
+      <c r="F10" s="13">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>5.5</v>
+      </c>
+      <c r="D13">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1.9</v>
+      </c>
+      <c r="D14">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.9</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>8.5</v>
+      </c>
+      <c r="D17">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>